<commit_message>
Added liquor cabinet display widget to index
</commit_message>
<xml_diff>
--- a/lib/seeds/ingredients.xlsx
+++ b/lib/seeds/ingredients.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carterbacon/code/ruby/cocktail/lib/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B8574E4-7796-414E-8633-EE6FF0D75592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA418D4F-2DAE-A54A-9550-5E4F99AE3F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42820" yWindow="20" windowWidth="28040" windowHeight="17440" xr2:uid="{E1247D6A-5AEA-5848-A265-AE248DEDC358}"/>
+    <workbookView xWindow="11020" yWindow="1340" windowWidth="23940" windowHeight="17440" xr2:uid="{E1247D6A-5AEA-5848-A265-AE248DEDC358}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tools" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="178">
   <si>
     <t>display_name</t>
   </si>
@@ -63,9 +62,6 @@
     <t>Syrup</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Modifier</t>
   </si>
   <si>
@@ -150,15 +146,6 @@
     <t>Shaved Ice</t>
   </si>
   <si>
-    <t>Straw</t>
-  </si>
-  <si>
-    <t>Glass Tube</t>
-  </si>
-  <si>
-    <t>Shaker</t>
-  </si>
-  <si>
     <t>Maraschino Cherries</t>
   </si>
   <si>
@@ -577,6 +564,12 @@
   </si>
   <si>
     <t>Gooseberry Jucie</t>
+  </si>
+  <si>
+    <t>Vodka</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -939,10 +932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71F2C7C-1CAF-7642-BD55-BC2EE4CAB643}">
-  <dimension ref="A1:G148"/>
+  <dimension ref="A1:G149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -953,7 +946,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -971,469 +964,469 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" t="s">
         <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" t="s">
         <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>129</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C22" t="s">
         <v>12</v>
-      </c>
-      <c r="B22" t="s">
-        <v>178</v>
-      </c>
-      <c r="C22" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" t="s">
         <v>12</v>
-      </c>
-      <c r="B24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s">
         <v>12</v>
-      </c>
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
         <v>23</v>
-      </c>
-      <c r="C30" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" t="s">
         <v>12</v>
-      </c>
-      <c r="B32" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" t="s">
         <v>12</v>
-      </c>
-      <c r="B33" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
         <v>12</v>
-      </c>
-      <c r="B34" t="s">
-        <v>98</v>
-      </c>
-      <c r="C34" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>171</v>
+      </c>
+      <c r="C35" t="s">
         <v>12</v>
-      </c>
-      <c r="B35" t="s">
-        <v>175</v>
-      </c>
-      <c r="C35" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" t="s">
         <v>12</v>
-      </c>
-      <c r="B36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C40" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C41" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C42" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C43" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F43">
         <v>0.25</v>
@@ -1441,24 +1434,24 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F45">
         <v>0.4</v>
@@ -1466,35 +1459,35 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C46" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C47" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F48">
         <v>0.45</v>
@@ -1502,24 +1495,24 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C49" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C50" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F50">
         <v>0.12</v>
@@ -1527,13 +1520,13 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C51" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F51">
         <v>0.45</v>
@@ -1541,13 +1534,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F52">
         <v>0.12</v>
@@ -1555,13 +1548,13 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C53" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F53">
         <v>0.55000000000000004</v>
@@ -1569,13 +1562,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C54" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F54">
         <v>0.12</v>
@@ -1583,13 +1576,13 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F55">
         <v>0.14099999999999999</v>
@@ -1597,24 +1590,24 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C56" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C57" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F57">
         <v>0.18</v>
@@ -1622,13 +1615,13 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C58" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F58">
         <v>0.18</v>
@@ -1636,13 +1629,13 @@
     </row>
     <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C59" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F59">
         <v>0.15</v>
@@ -1650,13 +1643,13 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C60" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F60">
         <v>0.16</v>
@@ -1664,19 +1657,19 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C61" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D61" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E61" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F61">
         <v>0.39</v>
@@ -1684,35 +1677,35 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C62" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C63" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C64" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F64">
         <v>0.55000000000000004</v>
@@ -1720,35 +1713,35 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C67" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F67">
         <v>0.4</v>
@@ -1756,79 +1749,79 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C68" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B69" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C72" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B73" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C73" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B74" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C74" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F74">
         <v>0.19</v>
@@ -1836,13 +1829,13 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C75" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F75">
         <v>0.32</v>
@@ -1850,35 +1843,35 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B76" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C76" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B77" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C77" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B78" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C78" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F78">
         <v>0.45</v>
@@ -1886,46 +1879,46 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C80" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B81" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C81" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B82" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C82" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F82">
         <v>0.2</v>
@@ -1933,24 +1926,24 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B83" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C83" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B84" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C84" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F84">
         <v>0.55000000000000004</v>
@@ -1958,35 +1951,35 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B85" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C85" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C86" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B87" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C87" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F87">
         <v>0.13500000000000001</v>
@@ -1994,13 +1987,13 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B88" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C88" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F88">
         <v>0.12</v>
@@ -2008,13 +2001,13 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B89" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C89" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F89">
         <v>0.13</v>
@@ -2022,35 +2015,35 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B90" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C90" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B91" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C91" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C92" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F92">
         <v>0.18</v>
@@ -2058,24 +2051,24 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B93" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C93" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B94" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C94" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F94">
         <v>0.12</v>
@@ -2083,13 +2076,13 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B95" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C95" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F95">
         <v>0.16</v>
@@ -2097,35 +2090,35 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B96" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C96" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B97" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C97" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B98" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C98" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F98">
         <v>0.55000000000000004</v>
@@ -2133,46 +2126,46 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B99" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C99" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B100" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C100" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>8</v>
+      </c>
+      <c r="B101" t="s">
         <v>9</v>
       </c>
-      <c r="B101" t="s">
-        <v>10</v>
-      </c>
       <c r="C101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B102" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C102" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F102">
         <v>0.1</v>
@@ -2180,13 +2173,13 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B103" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C103" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F103">
         <v>0.55000000000000004</v>
@@ -2194,13 +2187,13 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B104" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C104" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F104">
         <v>0.6</v>
@@ -2208,13 +2201,13 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B105" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C105" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F105">
         <v>0.4</v>
@@ -2222,13 +2215,13 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>13</v>
+      </c>
+      <c r="B106" t="s">
+        <v>143</v>
+      </c>
+      <c r="C106" t="s">
         <v>14</v>
-      </c>
-      <c r="B106" t="s">
-        <v>147</v>
-      </c>
-      <c r="C106" t="s">
-        <v>15</v>
       </c>
       <c r="F106">
         <v>0.4</v>
@@ -2236,13 +2229,13 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B107" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C107" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F107">
         <v>0.4</v>
@@ -2250,13 +2243,13 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>13</v>
+      </c>
+      <c r="B108" t="s">
         <v>14</v>
       </c>
-      <c r="B108" t="s">
-        <v>15</v>
-      </c>
       <c r="C108" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F108">
         <v>0.47499999999999998</v>
@@ -2264,13 +2257,13 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>13</v>
+      </c>
+      <c r="B109" t="s">
+        <v>100</v>
+      </c>
+      <c r="C109" t="s">
         <v>14</v>
-      </c>
-      <c r="B109" t="s">
-        <v>104</v>
-      </c>
-      <c r="C109" t="s">
-        <v>15</v>
       </c>
       <c r="F109">
         <v>0.4</v>
@@ -2278,13 +2271,13 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B110" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C110" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F110">
         <v>0.4</v>
@@ -2292,13 +2285,13 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B111" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C111" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F111">
         <v>0.4</v>
@@ -2306,13 +2299,13 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B112" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C112" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F112">
         <v>0.4</v>
@@ -2320,19 +2313,19 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B113" t="s">
+        <v>31</v>
+      </c>
+      <c r="C113" t="s">
         <v>32</v>
       </c>
-      <c r="C113" t="s">
-        <v>33</v>
-      </c>
       <c r="D113" t="s">
+        <v>29</v>
+      </c>
+      <c r="E113" t="s">
         <v>30</v>
-      </c>
-      <c r="E113" t="s">
-        <v>31</v>
       </c>
       <c r="F113">
         <v>0.4</v>
@@ -2340,13 +2333,13 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B114" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C114" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F114">
         <v>0.4</v>
@@ -2354,13 +2347,13 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B115" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C115" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F115">
         <v>0.4</v>
@@ -2368,24 +2361,24 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B116" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C116" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B117" t="s">
+        <v>15</v>
+      </c>
+      <c r="C117" t="s">
         <v>16</v>
-      </c>
-      <c r="C117" t="s">
-        <v>17</v>
       </c>
       <c r="F117">
         <v>0.63</v>
@@ -2393,13 +2386,13 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B118" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C118" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F118">
         <v>0.4</v>
@@ -2407,13 +2400,13 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B119" t="s">
+        <v>104</v>
+      </c>
+      <c r="C119" t="s">
         <v>14</v>
-      </c>
-      <c r="B119" t="s">
-        <v>108</v>
-      </c>
-      <c r="C119" t="s">
-        <v>15</v>
       </c>
       <c r="F119">
         <v>0.4</v>
@@ -2421,13 +2414,13 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B120" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C120" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F120" s="2">
         <v>0.4</v>
@@ -2435,13 +2428,13 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B121" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C121" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F121">
         <v>0.4</v>
@@ -2449,13 +2442,13 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B122" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C122" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F122">
         <v>0.5</v>
@@ -2463,13 +2456,13 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B123" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C123" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F123">
         <v>0.4</v>
@@ -2477,13 +2470,13 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B124" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C124" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F124">
         <v>0.4</v>
@@ -2491,13 +2484,13 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B125" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C125" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F125">
         <v>0.4</v>
@@ -2505,13 +2498,13 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B126" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C126" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F126">
         <v>0.4</v>
@@ -2519,13 +2512,13 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B127" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C127" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F127">
         <v>0.4</v>
@@ -2533,13 +2526,13 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B128" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C128" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F128">
         <v>0.4</v>
@@ -2547,27 +2540,30 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B129" t="s">
-        <v>26</v>
+        <v>176</v>
       </c>
       <c r="C129" t="s">
-        <v>26</v>
+        <v>176</v>
       </c>
       <c r="F129">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B130" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="C130" t="s">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="F130">
+        <v>0.45</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
@@ -2575,10 +2571,10 @@
         <v>6</v>
       </c>
       <c r="B131" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="C131" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
@@ -2586,7 +2582,7 @@
         <v>6</v>
       </c>
       <c r="B132" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="C132" t="s">
         <v>7</v>
@@ -2597,7 +2593,7 @@
         <v>6</v>
       </c>
       <c r="B133" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="C133" t="s">
         <v>7</v>
@@ -2608,10 +2604,10 @@
         <v>6</v>
       </c>
       <c r="B134" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C134" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
@@ -2619,10 +2615,10 @@
         <v>6</v>
       </c>
       <c r="B135" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C135" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
@@ -2630,10 +2626,10 @@
         <v>6</v>
       </c>
       <c r="B136" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="C136" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
@@ -2641,10 +2637,10 @@
         <v>6</v>
       </c>
       <c r="B137" t="s">
-        <v>177</v>
+        <v>123</v>
       </c>
       <c r="C137" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
@@ -2652,10 +2648,10 @@
         <v>6</v>
       </c>
       <c r="B138" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="C138" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
@@ -2663,10 +2659,10 @@
         <v>6</v>
       </c>
       <c r="B139" t="s">
-        <v>128</v>
+        <v>65</v>
       </c>
       <c r="C139" t="s">
-        <v>128</v>
+        <v>6</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
@@ -2674,10 +2670,10 @@
         <v>6</v>
       </c>
       <c r="B140" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="C140" t="s">
-        <v>7</v>
+        <v>124</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
@@ -2685,7 +2681,7 @@
         <v>6</v>
       </c>
       <c r="B141" t="s">
-        <v>168</v>
+        <v>53</v>
       </c>
       <c r="C141" t="s">
         <v>7</v>
@@ -2696,10 +2692,10 @@
         <v>6</v>
       </c>
       <c r="B142" t="s">
-        <v>22</v>
+        <v>164</v>
       </c>
       <c r="C142" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
@@ -2707,10 +2703,10 @@
         <v>6</v>
       </c>
       <c r="B143" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C143" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
@@ -2718,7 +2714,7 @@
         <v>6</v>
       </c>
       <c r="B144" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="C144" t="s">
         <v>7</v>
@@ -2729,7 +2725,7 @@
         <v>6</v>
       </c>
       <c r="B145" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C145" t="s">
         <v>7</v>
@@ -2740,10 +2736,10 @@
         <v>6</v>
       </c>
       <c r="B146" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C146" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
@@ -2751,7 +2747,7 @@
         <v>6</v>
       </c>
       <c r="B147" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="C147" t="s">
         <v>6</v>
@@ -2762,52 +2758,28 @@
         <v>6</v>
       </c>
       <c r="B148" t="s">
-        <v>167</v>
+        <v>101</v>
       </c>
       <c r="C148" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>6</v>
+      </c>
+      <c r="B149" t="s">
+        <v>163</v>
+      </c>
+      <c r="C149" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G148">
-    <sortCondition ref="A2:A148"/>
-    <sortCondition ref="B2:B148"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G149">
+    <sortCondition ref="A2:A149"/>
+    <sortCondition ref="B2:B149"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D49B1A0-AD21-E54D-BFA4-8273401C6F7D}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>